<commit_message>
updated dashboards script and more
</commit_message>
<xml_diff>
--- a/master rebuilding stream list good.xlsx
+++ b/master rebuilding stream list good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\Documents\R\rebuilding_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24389188-46D7-4B14-8275-4226DFA09ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F053ADBB-1530-49EF-9AFE-2E018661E4F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11640" windowHeight="7970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,15 @@
     <sheet name="master rebuilding stream list" sheetId="1" r:id="rId1"/>
     <sheet name="Chinook" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chinook!$A$1:$U$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="385">
   <si>
     <t>Species</t>
   </si>
@@ -560,9 +563,6 @@
     <t>Englishman R</t>
   </si>
   <si>
-    <t>Bedwell R, Bedwell Est</t>
-  </si>
-  <si>
     <t>Elaho R</t>
   </si>
   <si>
@@ -593,9 +593,6 @@
     <t>52108,52118</t>
   </si>
   <si>
-    <t>Kennedy R low,Kennedy R Up</t>
-  </si>
-  <si>
     <t>Kilbella River</t>
   </si>
   <si>
@@ -1097,9 +1094,6 @@
     <t>GOLD RIVER</t>
   </si>
   <si>
-    <t>Gold R, Gold Est, Muchalat Lk</t>
-  </si>
-  <si>
     <t>Kilbella R,Kilbella Bay</t>
   </si>
   <si>
@@ -1143,6 +1137,48 @@
   </si>
   <si>
     <t>45190,52318,52328</t>
+  </si>
+  <si>
+    <t>Bedwell R,Bedwell Est</t>
+  </si>
+  <si>
+    <t>Clemens Cr</t>
+  </si>
+  <si>
+    <t>41348</t>
+  </si>
+  <si>
+    <t>Gold R,Gold Est,Muchalat Lk</t>
+  </si>
+  <si>
+    <t>Kennedy R Low,Kennedy R Up</t>
+  </si>
+  <si>
+    <t>ts</t>
+  </si>
+  <si>
+    <t>nos</t>
+  </si>
+  <si>
+    <t>wild</t>
+  </si>
+  <si>
+    <t>not enough esc data</t>
+  </si>
+  <si>
+    <t>no enh cont/pni data</t>
+  </si>
+  <si>
+    <t>only 2 pnos data points</t>
+  </si>
+  <si>
+    <t>BEDWELL SYSTEM</t>
+  </si>
+  <si>
+    <t>SAN JUAN RIVER</t>
+  </si>
+  <si>
+    <t>analysis.sys.link</t>
   </si>
 </sst>
 </file>
@@ -1656,12 +1692,13 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3095,11 +3132,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S46"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="31" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3107,17 +3147,18 @@
     <col min="3" max="3" width="19.26953125" customWidth="1"/>
     <col min="4" max="4" width="9.453125" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" customWidth="1"/>
-    <col min="6" max="6" width="24.26953125" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.453125" customWidth="1"/>
-    <col min="9" max="10" width="12.7265625" customWidth="1"/>
-    <col min="11" max="11" width="7.26953125" customWidth="1"/>
-    <col min="12" max="12" width="17.1796875" customWidth="1"/>
-    <col min="13" max="13" width="27.1796875" customWidth="1"/>
-    <col min="14" max="16" width="22.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="24.26953125" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.453125" customWidth="1"/>
+    <col min="10" max="11" width="12.7265625" customWidth="1"/>
+    <col min="12" max="12" width="7.26953125" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" customWidth="1"/>
+    <col min="14" max="14" width="27.1796875" customWidth="1"/>
+    <col min="15" max="17" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3134,208 +3175,220 @@
         <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" t="s">
-        <v>223</v>
-      </c>
       <c r="I1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" t="s">
         <v>114</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>153</v>
       </c>
-      <c r="K1" t="s">
-        <v>263</v>
-      </c>
       <c r="L1" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="M1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="N1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="O1" t="s">
-        <v>311</v>
+        <v>212</v>
       </c>
       <c r="P1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="Q1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R1" t="s">
         <v>106</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>107</v>
       </c>
-      <c r="S1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T1" t="s">
+        <v>358</v>
+      </c>
+      <c r="U1" t="s">
+        <v>376</v>
+      </c>
+      <c r="V1" t="s">
+        <v>377</v>
+      </c>
+      <c r="W1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>249</v>
       </c>
       <c r="D2">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="1">
-        <v>50034</v>
-      </c>
-      <c r="H2" t="s">
-        <v>113</v>
+      <c r="G2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>250</v>
       </c>
       <c r="J2" t="s">
-        <v>115</v>
+        <v>245</v>
       </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="M2" t="s">
-        <v>268</v>
-      </c>
-      <c r="O2" t="s">
-        <v>104</v>
+        <v>244</v>
+      </c>
+      <c r="N2" t="s">
+        <v>243</v>
       </c>
       <c r="P2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="Q2" t="s">
-        <v>117</v>
+        <v>244</v>
       </c>
       <c r="R2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>269</v>
       </c>
       <c r="D3">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>104</v>
       </c>
-      <c r="F3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="H3" t="s">
-        <v>128</v>
+      <c r="G3" t="s">
+        <v>268</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="J3" t="s">
-        <v>122</v>
+        <v>245</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="L3" t="s">
-        <v>179</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="O3" t="s">
-        <v>104</v>
+        <v>104</v>
+      </c>
+      <c r="M3" t="s">
+        <v>270</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="P3" t="s">
-        <v>343</v>
+        <v>104</v>
       </c>
       <c r="Q3" t="s">
-        <v>104</v>
+        <v>270</v>
       </c>
       <c r="R3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>104</v>
       </c>
-      <c r="F4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H4" t="s">
-        <v>129</v>
+      <c r="G4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="I4" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="J4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K4" t="s">
+        <v>240</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" t="s">
+        <v>347</v>
+      </c>
+      <c r="N4" t="s">
+        <v>241</v>
+      </c>
+      <c r="P4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q4" t="s">
         <v>342</v>
       </c>
-      <c r="K4" t="s">
-        <v>104</v>
-      </c>
-      <c r="L4" t="s">
-        <v>345</v>
-      </c>
-      <c r="M4" t="s">
-        <v>346</v>
-      </c>
-      <c r="O4" t="s">
-        <v>104</v>
-      </c>
-      <c r="P4" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>104</v>
-      </c>
       <c r="R4" t="s">
+        <v>104</v>
+      </c>
+      <c r="S4" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -3343,52 +3396,52 @@
         <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D5">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>104</v>
       </c>
-      <c r="F5" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" t="s">
-        <v>140</v>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="I5" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
-        <v>242</v>
+        <v>133</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>349</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s">
-        <v>243</v>
-      </c>
-      <c r="O5" t="s">
-        <v>104</v>
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>266</v>
       </c>
       <c r="P5" t="s">
-        <v>344</v>
+        <v>104</v>
       </c>
       <c r="Q5" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="R5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -3396,52 +3449,52 @@
         <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D6">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>104</v>
       </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="H6" t="s">
-        <v>113</v>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="I6" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="J6" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="K6" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s">
-        <v>268</v>
-      </c>
-      <c r="O6" t="s">
-        <v>104</v>
+        <v>38</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>351</v>
       </c>
       <c r="P6" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="Q6" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="R6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -3449,7 +3502,7 @@
         <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="D7">
         <v>17</v>
@@ -3457,633 +3510,666 @@
       <c r="E7" t="s">
         <v>104</v>
       </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" t="s">
-        <v>146</v>
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="J7" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="K7" t="s">
-        <v>104</v>
+        <v>177</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="O7" t="s">
-        <v>104</v>
+        <v>104</v>
+      </c>
+      <c r="M7" t="s">
+        <v>178</v>
+      </c>
+      <c r="N7" t="s">
+        <v>253</v>
+      </c>
+      <c r="O7">
+        <v>1998</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="D8">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>104</v>
       </c>
-      <c r="F8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="1">
-        <v>46851</v>
-      </c>
-      <c r="H8" t="s">
-        <v>120</v>
+      <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="I8" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="J8" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
       <c r="K8" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="L8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="M8" t="s">
-        <v>228</v>
-      </c>
-      <c r="O8" t="s">
-        <v>104</v>
+        <v>224</v>
+      </c>
+      <c r="N8" t="s">
+        <v>223</v>
+      </c>
+      <c r="O8">
+        <v>1981</v>
       </c>
       <c r="P8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q8" t="s">
-        <v>104</v>
+        <v>361</v>
       </c>
       <c r="R8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S8" t="s">
+        <v>361</v>
+      </c>
+      <c r="T8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>219</v>
       </c>
       <c r="D9">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" t="s">
-        <v>151</v>
+      <c r="G9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="K9" t="s">
-        <v>104</v>
-      </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+      <c r="L9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" t="s">
+        <v>220</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="P9" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>220</v>
+      </c>
+      <c r="R9" t="s">
+        <v>104</v>
+      </c>
+      <c r="S9" t="s">
+        <v>362</v>
+      </c>
+      <c r="T9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>237</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>104</v>
       </c>
-      <c r="F10" t="s">
-        <v>158</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H10" t="s">
-        <v>160</v>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="I10" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="J10" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="K10" t="s">
-        <v>104</v>
+        <v>240</v>
       </c>
       <c r="L10" t="s">
-        <v>351</v>
+        <v>104</v>
       </c>
       <c r="M10" t="s">
-        <v>354</v>
-      </c>
-      <c r="N10">
-        <v>1988</v>
-      </c>
-      <c r="O10" t="s">
+        <v>242</v>
+      </c>
+      <c r="N10" t="s">
+        <v>241</v>
+      </c>
+      <c r="P10" t="s">
         <v>172</v>
       </c>
-      <c r="Q10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R10" t="s">
+        <v>104</v>
+      </c>
+      <c r="S10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
         <v>104</v>
       </c>
-      <c r="F11" t="s">
-        <v>164</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H11" t="s">
-        <v>128</v>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="I11" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="J11" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="K11" t="s">
-        <v>104</v>
+        <v>177</v>
       </c>
       <c r="L11" t="s">
-        <v>290</v>
-      </c>
-      <c r="N11">
-        <v>1997</v>
-      </c>
-      <c r="O11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" t="s">
+        <v>254</v>
+      </c>
+      <c r="N11" t="s">
+        <v>253</v>
+      </c>
+      <c r="P11" t="s">
         <v>172</v>
       </c>
-      <c r="Q11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R11" t="s">
+        <v>104</v>
+      </c>
+      <c r="S11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="D12">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>104</v>
       </c>
-      <c r="F12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="1">
-        <v>46196</v>
-      </c>
-      <c r="H12" t="s">
-        <v>119</v>
+      <c r="G12" t="s">
+        <v>272</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="I12" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J12" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="K12" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s">
-        <v>108</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="O12" t="s">
-        <v>104</v>
+        <v>104</v>
+      </c>
+      <c r="M12" t="s">
+        <v>275</v>
+      </c>
+      <c r="N12" t="s">
+        <v>241</v>
       </c>
       <c r="P12" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="D13">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
-        <v>167</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H13" t="s">
-        <v>128</v>
+      <c r="G13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="1">
+        <v>50034</v>
       </c>
       <c r="I13" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="J13" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="K13" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L13" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
       <c r="M13" t="s">
-        <v>290</v>
-      </c>
-      <c r="N13">
-        <v>1990</v>
-      </c>
-      <c r="O13" t="s">
-        <v>172</v>
+        <v>111</v>
+      </c>
+      <c r="N13" t="s">
+        <v>266</v>
+      </c>
+      <c r="P13" t="s">
+        <v>104</v>
       </c>
       <c r="Q13" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="R13" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+      <c r="S13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="D14">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H14" t="s">
-        <v>113</v>
+        <v>104</v>
+      </c>
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="1">
+        <v>46851</v>
       </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="J14" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="K14" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="L14" t="s">
-        <v>180</v>
-      </c>
-      <c r="O14" t="s">
-        <v>172</v>
+        <v>104</v>
+      </c>
+      <c r="M14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N14" t="s">
+        <v>226</v>
+      </c>
+      <c r="P14" t="s">
+        <v>104</v>
       </c>
       <c r="Q14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+      <c r="R14" t="s">
+        <v>104</v>
+      </c>
+      <c r="S14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="D15">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>104</v>
       </c>
-      <c r="F15" t="s">
-        <v>174</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" t="s">
-        <v>176</v>
+      <c r="G15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="I15" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="J15" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="K15" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="L15" t="s">
-        <v>178</v>
-      </c>
-      <c r="M15" t="s">
-        <v>255</v>
-      </c>
-      <c r="N15">
-        <v>1998</v>
-      </c>
-      <c r="O15" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>104</v>
-      </c>
-      <c r="R15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D16">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>104</v>
       </c>
-      <c r="F16" t="s">
-        <v>188</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H16" t="s">
-        <v>128</v>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="1">
+        <v>46196</v>
       </c>
       <c r="I16" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="J16" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="K16" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="L16" t="s">
-        <v>190</v>
+        <v>104</v>
       </c>
       <c r="M16" t="s">
-        <v>290</v>
-      </c>
-      <c r="O16" t="s">
-        <v>172</v>
+        <v>108</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="P16" t="s">
+        <v>104</v>
       </c>
       <c r="Q16" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="R16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>104</v>
       </c>
-      <c r="F17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H17" t="s">
-        <v>160</v>
+      <c r="G17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="I17" t="s">
-        <v>161</v>
+        <v>209</v>
       </c>
       <c r="J17" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="K17" t="s">
-        <v>104</v>
+        <v>211</v>
       </c>
       <c r="L17" t="s">
-        <v>359</v>
+        <v>104</v>
       </c>
       <c r="M17" t="s">
-        <v>354</v>
-      </c>
-      <c r="N17">
-        <v>1986</v>
-      </c>
-      <c r="O17" t="s">
-        <v>172</v>
+        <v>215</v>
+      </c>
+      <c r="N17" t="s">
+        <v>357</v>
+      </c>
+      <c r="O17">
+        <v>1996</v>
+      </c>
+      <c r="P17" t="s">
+        <v>104</v>
       </c>
       <c r="Q17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="R17" t="s">
+        <v>104</v>
+      </c>
+      <c r="S17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
-      <c r="F18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H18" t="s">
-        <v>197</v>
+      <c r="G18" t="s">
+        <v>228</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="I18" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="J18" t="s">
-        <v>199</v>
+        <v>131</v>
       </c>
       <c r="K18" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="L18" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="M18" t="s">
-        <v>321</v>
-      </c>
-      <c r="N18">
-        <v>1984</v>
-      </c>
-      <c r="O18" t="s">
+        <v>227</v>
+      </c>
+      <c r="N18" t="s">
+        <v>226</v>
+      </c>
+      <c r="O18">
+        <v>2014</v>
+      </c>
+      <c r="P18" t="s">
         <v>172</v>
       </c>
-      <c r="Q18" t="s">
-        <v>104</v>
-      </c>
       <c r="R18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="D19">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>104</v>
       </c>
-      <c r="F19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H19" t="s">
-        <v>113</v>
+      <c r="G19" t="s">
+        <v>233</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="I19" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="J19" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="K19" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="L19" t="s">
-        <v>216</v>
+        <v>104</v>
       </c>
       <c r="M19" t="s">
-        <v>268</v>
-      </c>
-      <c r="O19" t="s">
-        <v>104</v>
+        <v>236</v>
+      </c>
+      <c r="N19" t="s">
+        <v>235</v>
+      </c>
+      <c r="O19">
+        <v>1985</v>
       </c>
       <c r="P19" t="s">
-        <v>216</v>
+        <v>104</v>
       </c>
       <c r="Q19" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="R19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -4091,7 +4177,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="D20">
         <v>29</v>
@@ -4099,665 +4185,659 @@
       <c r="E20" t="s">
         <v>104</v>
       </c>
-      <c r="F20" t="s">
-        <v>209</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H20" t="s">
-        <v>211</v>
+      <c r="G20" t="s">
+        <v>257</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="I20" t="s">
-        <v>212</v>
+        <v>258</v>
       </c>
       <c r="J20" t="s">
-        <v>213</v>
+        <v>259</v>
       </c>
       <c r="K20" t="s">
-        <v>104</v>
+        <v>260</v>
       </c>
       <c r="L20" t="s">
-        <v>217</v>
-      </c>
-      <c r="M20" t="s">
-        <v>360</v>
-      </c>
-      <c r="N20">
-        <v>1996</v>
-      </c>
-      <c r="O20" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="P20" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="D21">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="F21" t="s">
-        <v>231</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="H21" t="s">
-        <v>197</v>
+      <c r="G21" t="s">
+        <v>272</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="I21" t="s">
-        <v>198</v>
+        <v>279</v>
       </c>
       <c r="J21" t="s">
-        <v>199</v>
+        <v>277</v>
       </c>
       <c r="K21" t="s">
-        <v>104</v>
+        <v>278</v>
       </c>
       <c r="L21" t="s">
-        <v>220</v>
-      </c>
-      <c r="O21" t="s">
-        <v>172</v>
+        <v>104</v>
+      </c>
+      <c r="M21" t="s">
+        <v>276</v>
+      </c>
+      <c r="N21" t="s">
+        <v>274</v>
+      </c>
+      <c r="P21" t="s">
+        <v>104</v>
       </c>
       <c r="Q21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+      <c r="R21" t="s">
+        <v>104</v>
+      </c>
+      <c r="S21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>221</v>
+        <v>290</v>
       </c>
       <c r="D22">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
         <v>104</v>
       </c>
-      <c r="F22" t="s">
-        <v>186</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H22" t="s">
-        <v>185</v>
+      <c r="G22" t="s">
+        <v>291</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>292</v>
       </c>
       <c r="I22" t="s">
-        <v>182</v>
+        <v>293</v>
       </c>
       <c r="J22" t="s">
-        <v>183</v>
+        <v>294</v>
       </c>
       <c r="K22" t="s">
-        <v>104</v>
+        <v>295</v>
       </c>
       <c r="L22" t="s">
-        <v>226</v>
+        <v>104</v>
       </c>
       <c r="M22" t="s">
-        <v>225</v>
-      </c>
-      <c r="N22">
-        <v>1981</v>
-      </c>
-      <c r="O22" t="s">
-        <v>104</v>
+        <v>296</v>
+      </c>
+      <c r="N22" t="s">
+        <v>297</v>
       </c>
       <c r="P22" t="s">
-        <v>364</v>
+        <v>104</v>
       </c>
       <c r="Q22" t="s">
-        <v>104</v>
+        <v>296</v>
       </c>
       <c r="R22" t="s">
-        <v>364</v>
+        <v>104</v>
       </c>
       <c r="S22" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>221</v>
+        <v>305</v>
       </c>
       <c r="D23">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
         <v>104</v>
       </c>
-      <c r="F23" t="s">
-        <v>186</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H23" t="s">
-        <v>146</v>
+      <c r="G23" t="s">
+        <v>306</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="J23" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="K23" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="L23" t="s">
-        <v>222</v>
+        <v>104</v>
       </c>
       <c r="M23" t="s">
-        <v>353</v>
-      </c>
-      <c r="O23" t="s">
-        <v>104</v>
+        <v>307</v>
+      </c>
+      <c r="N23" t="s">
+        <v>235</v>
       </c>
       <c r="P23" t="s">
-        <v>222</v>
+        <v>104</v>
       </c>
       <c r="Q23" t="s">
-        <v>104</v>
+        <v>307</v>
       </c>
       <c r="R23" t="s">
-        <v>365</v>
+        <v>104</v>
       </c>
       <c r="S23" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>324</v>
       </c>
       <c r="C24" t="s">
-        <v>227</v>
+        <v>323</v>
       </c>
       <c r="D24">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="F24" t="s">
-        <v>230</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H24" t="s">
-        <v>120</v>
+      <c r="G24" t="s">
+        <v>327</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="I24" t="s">
-        <v>131</v>
+        <v>332</v>
       </c>
       <c r="J24" t="s">
-        <v>123</v>
+        <v>333</v>
       </c>
       <c r="K24" t="s">
-        <v>104</v>
+        <v>334</v>
       </c>
       <c r="L24" t="s">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="M24" t="s">
-        <v>228</v>
-      </c>
-      <c r="N24">
-        <v>2014</v>
-      </c>
-      <c r="O24" t="s">
+        <v>338</v>
+      </c>
+      <c r="N24" t="s">
+        <v>339</v>
+      </c>
+      <c r="P24" t="s">
         <v>172</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="D25">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
         <v>104</v>
       </c>
-      <c r="F25" t="s">
-        <v>235</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H25" t="s">
-        <v>119</v>
+      <c r="G25" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="I25" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="J25" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="K25" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="L25" t="s">
-        <v>238</v>
+        <v>104</v>
       </c>
       <c r="M25" t="s">
-        <v>237</v>
-      </c>
-      <c r="N25">
-        <v>1985</v>
-      </c>
-      <c r="O25" t="s">
-        <v>104</v>
+        <v>349</v>
+      </c>
+      <c r="N25" t="s">
+        <v>352</v>
+      </c>
+      <c r="O25">
+        <v>1988</v>
       </c>
       <c r="P25" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R25" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C26" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="D26">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>104</v>
       </c>
-      <c r="F26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H26" t="s">
-        <v>140</v>
+      <c r="G26" t="s">
+        <v>190</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="I26" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="J26" t="s">
-        <v>242</v>
+        <v>161</v>
       </c>
       <c r="K26" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="L26" t="s">
-        <v>244</v>
+        <v>104</v>
       </c>
       <c r="M26" t="s">
-        <v>243</v>
-      </c>
-      <c r="O26" t="s">
+        <v>356</v>
+      </c>
+      <c r="N26" t="s">
+        <v>352</v>
+      </c>
+      <c r="O26">
+        <v>1986</v>
+      </c>
+      <c r="P26" t="s">
         <v>172</v>
       </c>
-      <c r="Q26" t="s">
-        <v>104</v>
-      </c>
       <c r="R26" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>240</v>
+        <v>135</v>
       </c>
       <c r="C27" t="s">
-        <v>251</v>
+        <v>125</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
         <v>104</v>
       </c>
-      <c r="F27" t="s">
-        <v>249</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H27" t="s">
-        <v>252</v>
+      <c r="G27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="I27" t="s">
-        <v>247</v>
+        <v>129</v>
       </c>
       <c r="J27" t="s">
-        <v>248</v>
+        <v>130</v>
       </c>
       <c r="K27" t="s">
-        <v>104</v>
+        <v>340</v>
       </c>
       <c r="L27" t="s">
-        <v>246</v>
+        <v>104</v>
       </c>
       <c r="M27" t="s">
-        <v>245</v>
-      </c>
-      <c r="O27" t="s">
-        <v>104</v>
+        <v>343</v>
+      </c>
+      <c r="N27" t="s">
+        <v>344</v>
       </c>
       <c r="P27" t="s">
-        <v>246</v>
+        <v>104</v>
       </c>
       <c r="Q27" t="s">
-        <v>104</v>
+        <v>345</v>
       </c>
       <c r="R27" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
-        <v>253</v>
+        <v>171</v>
       </c>
       <c r="D28">
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="H28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I28" t="s">
-        <v>181</v>
+        <v>113</v>
       </c>
       <c r="J28" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="K28" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L28" t="s">
-        <v>256</v>
+        <v>104</v>
       </c>
       <c r="M28" t="s">
-        <v>255</v>
-      </c>
-      <c r="O28" t="s">
+        <v>179</v>
+      </c>
+      <c r="P28" t="s">
         <v>172</v>
       </c>
-      <c r="Q28" t="s">
-        <v>104</v>
-      </c>
       <c r="R28" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="C29" t="s">
-        <v>258</v>
+        <v>203</v>
       </c>
       <c r="D29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
         <v>104</v>
       </c>
-      <c r="F29" t="s">
-        <v>259</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="H29" t="s">
-        <v>260</v>
+      <c r="G29" t="s">
+        <v>204</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="I29" t="s">
-        <v>261</v>
+        <v>113</v>
       </c>
       <c r="J29" t="s">
-        <v>262</v>
+        <v>133</v>
       </c>
       <c r="K29" t="s">
-        <v>172</v>
-      </c>
-      <c r="O29" t="s">
-        <v>172</v>
+        <v>115</v>
+      </c>
+      <c r="L29" t="s">
+        <v>104</v>
+      </c>
+      <c r="M29" t="s">
+        <v>214</v>
+      </c>
+      <c r="N29" t="s">
+        <v>266</v>
+      </c>
+      <c r="P29" t="s">
+        <v>104</v>
       </c>
       <c r="Q29" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="R29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>240</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
         <v>104</v>
       </c>
-      <c r="F30" t="s">
-        <v>270</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H30" t="s">
-        <v>252</v>
+      <c r="G30" t="s">
+        <v>263</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="I30" t="s">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="J30" t="s">
-        <v>248</v>
+        <v>133</v>
       </c>
       <c r="K30" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L30" t="s">
-        <v>272</v>
+        <v>104</v>
       </c>
       <c r="M30" t="s">
-        <v>245</v>
-      </c>
-      <c r="O30" t="s">
-        <v>104</v>
+        <v>265</v>
+      </c>
+      <c r="N30" t="s">
+        <v>266</v>
       </c>
       <c r="P30" t="s">
-        <v>272</v>
+        <v>104</v>
       </c>
       <c r="Q30" t="s">
-        <v>104</v>
+        <v>265</v>
       </c>
       <c r="R30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
-        <v>273</v>
+        <v>311</v>
       </c>
       <c r="D31">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
         <v>104</v>
       </c>
-      <c r="F31" t="s">
-        <v>274</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="H31" t="s">
-        <v>140</v>
+      <c r="G31" t="s">
+        <v>312</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="I31" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="J31" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="K31" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="L31" t="s">
-        <v>277</v>
+        <v>104</v>
       </c>
       <c r="M31" t="s">
-        <v>243</v>
-      </c>
-      <c r="O31" t="s">
+        <v>313</v>
+      </c>
+      <c r="N31" t="s">
+        <v>266</v>
+      </c>
+      <c r="P31" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>315</v>
+      </c>
+      <c r="R31" t="s">
         <v>172</v>
       </c>
-      <c r="Q31" t="s">
-        <v>104</v>
-      </c>
-      <c r="R31" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="S31" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>283</v>
+        <v>121</v>
       </c>
       <c r="D32">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E32" t="s">
         <v>104</v>
       </c>
       <c r="F32" t="s">
-        <v>274</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H32" t="s">
-        <v>281</v>
+        <v>382</v>
+      </c>
+      <c r="G32" t="s">
+        <v>369</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="I32" t="s">
-        <v>279</v>
+        <v>128</v>
       </c>
       <c r="J32" t="s">
-        <v>280</v>
+        <v>134</v>
       </c>
       <c r="K32" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L32" t="s">
-        <v>278</v>
+        <v>104</v>
       </c>
       <c r="M32" t="s">
-        <v>276</v>
-      </c>
-      <c r="O32" t="s">
-        <v>104</v>
+        <v>371</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="O32">
+        <v>2009</v>
       </c>
       <c r="P32" t="s">
-        <v>278</v>
+        <v>104</v>
       </c>
       <c r="Q32" t="s">
-        <v>104</v>
+        <v>341</v>
       </c>
       <c r="R32" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S32" t="s">
+        <v>121</v>
+      </c>
+      <c r="U32" t="s">
+        <v>16</v>
+      </c>
+      <c r="V32" t="s">
+        <v>16</v>
+      </c>
+      <c r="W32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -4765,52 +4845,61 @@
         <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>284</v>
+        <v>163</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E33" t="s">
         <v>104</v>
       </c>
       <c r="F33" t="s">
-        <v>306</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H33" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" t="s">
+        <v>164</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I33" t="s">
         <v>128</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>134</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>122</v>
       </c>
-      <c r="K33" t="s">
-        <v>104</v>
-      </c>
       <c r="L33" t="s">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="M33" t="s">
-        <v>290</v>
-      </c>
-      <c r="O33" t="s">
-        <v>104</v>
+        <v>372</v>
+      </c>
+      <c r="N33" t="s">
+        <v>288</v>
+      </c>
+      <c r="O33">
+        <v>1997</v>
       </c>
       <c r="P33" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R33" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="U33" t="s">
+        <v>57</v>
+      </c>
+      <c r="V33" t="s">
+        <v>57</v>
+      </c>
+      <c r="W33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>99</v>
       </c>
@@ -4818,158 +4907,194 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>285</v>
+        <v>166</v>
       </c>
       <c r="D34">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
         <v>104</v>
       </c>
       <c r="F34" t="s">
-        <v>286</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="H34" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" t="s">
         <v>128</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" t="s">
+        <v>122</v>
+      </c>
+      <c r="L34" t="s">
+        <v>104</v>
+      </c>
+      <c r="M34" t="s">
+        <v>169</v>
+      </c>
+      <c r="N34" t="s">
         <v>288</v>
       </c>
-      <c r="J34" t="s">
-        <v>122</v>
-      </c>
-      <c r="K34" t="s">
-        <v>104</v>
-      </c>
-      <c r="L34" t="s">
-        <v>291</v>
-      </c>
-      <c r="M34" t="s">
-        <v>290</v>
-      </c>
-      <c r="O34" t="s">
-        <v>104</v>
+      <c r="O34">
+        <v>1990</v>
       </c>
       <c r="P34" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R34" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S34" t="s">
+        <v>353</v>
+      </c>
+      <c r="U34" t="s">
+        <v>16</v>
+      </c>
+      <c r="V34" t="s">
+        <v>57</v>
+      </c>
+      <c r="W34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>264</v>
+        <v>354</v>
       </c>
       <c r="D35">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E35" t="s">
         <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>265</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="H35" t="s">
-        <v>113</v>
+        <v>355</v>
+      </c>
+      <c r="G35" t="s">
+        <v>355</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="I35" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="J35" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="K35" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="L35" t="s">
-        <v>267</v>
+        <v>104</v>
       </c>
       <c r="M35" t="s">
-        <v>268</v>
-      </c>
-      <c r="O35" t="s">
-        <v>104</v>
+        <v>374</v>
+      </c>
+      <c r="N35" t="s">
+        <v>319</v>
+      </c>
+      <c r="O35">
+        <v>1983</v>
       </c>
       <c r="P35" t="s">
-        <v>267</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R35" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S35" t="s">
+        <v>354</v>
+      </c>
+      <c r="U35" t="s">
+        <v>16</v>
+      </c>
+      <c r="V35" t="s">
+        <v>16</v>
+      </c>
+      <c r="W35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>292</v>
+        <v>186</v>
       </c>
       <c r="D36">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E36" t="s">
         <v>104</v>
       </c>
-      <c r="F36" t="s">
-        <v>293</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H36" t="s">
-        <v>295</v>
+      <c r="G36" t="s">
+        <v>187</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="I36" t="s">
-        <v>296</v>
+        <v>128</v>
       </c>
       <c r="J36" t="s">
-        <v>297</v>
+        <v>134</v>
       </c>
       <c r="K36" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L36" t="s">
-        <v>298</v>
+        <v>104</v>
       </c>
       <c r="M36" t="s">
-        <v>299</v>
-      </c>
-      <c r="O36" t="s">
-        <v>104</v>
+        <v>375</v>
+      </c>
+      <c r="N36" t="s">
+        <v>288</v>
+      </c>
+      <c r="O36">
+        <v>1982</v>
       </c>
       <c r="P36" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R36" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S36" t="s">
+        <v>186</v>
+      </c>
+      <c r="U36" t="s">
+        <v>57</v>
+      </c>
+      <c r="V36" t="s">
+        <v>57</v>
+      </c>
+      <c r="W36" t="s">
+        <v>57</v>
+      </c>
+      <c r="X36" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -4977,158 +5102,194 @@
         <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>300</v>
+        <v>192</v>
       </c>
       <c r="D37">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
         <v>104</v>
       </c>
       <c r="F37" t="s">
-        <v>301</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H37" t="s">
-        <v>128</v>
+        <v>194</v>
+      </c>
+      <c r="G37" t="s">
+        <v>194</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="I37" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="J37" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="K37" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="L37" t="s">
-        <v>303</v>
+        <v>104</v>
       </c>
       <c r="M37" t="s">
-        <v>290</v>
-      </c>
-      <c r="O37" t="s">
-        <v>104</v>
+        <v>200</v>
+      </c>
+      <c r="N37" t="s">
+        <v>319</v>
+      </c>
+      <c r="O37">
+        <v>1984</v>
       </c>
       <c r="P37" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R37" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S37" t="s">
+        <v>192</v>
+      </c>
+      <c r="U37" t="s">
+        <v>16</v>
+      </c>
+      <c r="V37" t="s">
+        <v>16</v>
+      </c>
+      <c r="W37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>307</v>
+        <v>216</v>
       </c>
       <c r="D38">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E38" t="s">
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>308</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H38" t="s">
-        <v>119</v>
+        <v>229</v>
+      </c>
+      <c r="G38" t="s">
+        <v>229</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="I38" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="J38" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="K38" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="L38" t="s">
-        <v>309</v>
+        <v>104</v>
       </c>
       <c r="M38" t="s">
-        <v>237</v>
-      </c>
-      <c r="O38" t="s">
-        <v>104</v>
+        <v>218</v>
+      </c>
+      <c r="O38">
+        <v>1989</v>
       </c>
       <c r="P38" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="R38" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="U38" t="s">
+        <v>57</v>
+      </c>
+      <c r="V38" t="s">
+        <v>57</v>
+      </c>
+      <c r="W38" t="s">
+        <v>57</v>
+      </c>
+      <c r="X38" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="D39">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
         <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>314</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H39" t="s">
-        <v>113</v>
+        <v>383</v>
+      </c>
+      <c r="G39" t="s">
+        <v>304</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="I39" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J39" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="K39" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L39" t="s">
-        <v>315</v>
+        <v>104</v>
       </c>
       <c r="M39" t="s">
-        <v>268</v>
-      </c>
-      <c r="O39" t="s">
-        <v>104</v>
+        <v>287</v>
+      </c>
+      <c r="N39" t="s">
+        <v>288</v>
+      </c>
+      <c r="O39">
+        <v>1980</v>
       </c>
       <c r="P39" t="s">
-        <v>317</v>
+        <v>104</v>
       </c>
       <c r="Q39" t="s">
-        <v>172</v>
+        <v>368</v>
       </c>
       <c r="R39" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S39" t="s">
+        <v>282</v>
+      </c>
+      <c r="U39" t="s">
+        <v>16</v>
+      </c>
+      <c r="V39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -5136,49 +5297,67 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="D40">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
         <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>327</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="H40" t="s">
-        <v>197</v>
+        <v>284</v>
+      </c>
+      <c r="G40" t="s">
+        <v>284</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="I40" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="J40" t="s">
-        <v>199</v>
+        <v>286</v>
       </c>
       <c r="K40" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L40" t="s">
-        <v>320</v>
+        <v>104</v>
       </c>
       <c r="M40" t="s">
-        <v>321</v>
-      </c>
-      <c r="O40" t="s">
-        <v>172</v>
+        <v>289</v>
+      </c>
+      <c r="N40" t="s">
+        <v>288</v>
+      </c>
+      <c r="O40">
+        <v>1985</v>
+      </c>
+      <c r="P40" t="s">
+        <v>104</v>
       </c>
       <c r="Q40" t="s">
-        <v>104</v>
+        <v>366</v>
       </c>
       <c r="R40" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S40" t="s">
+        <v>283</v>
+      </c>
+      <c r="U40" t="s">
+        <v>16</v>
+      </c>
+      <c r="V40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -5186,43 +5365,67 @@
         <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>298</v>
       </c>
       <c r="D41">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E41" t="s">
         <v>104</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H41" t="s">
-        <v>197</v>
+        <v>299</v>
+      </c>
+      <c r="G41" t="s">
+        <v>299</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="I41" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="J41" t="s">
-        <v>199</v>
+        <v>134</v>
       </c>
       <c r="K41" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L41" t="s">
-        <v>203</v>
+        <v>104</v>
+      </c>
+      <c r="M41" t="s">
+        <v>301</v>
+      </c>
+      <c r="N41" t="s">
+        <v>288</v>
+      </c>
+      <c r="O41">
+        <v>1981</v>
+      </c>
+      <c r="P41" t="s">
+        <v>104</v>
       </c>
       <c r="Q41" t="s">
-        <v>104</v>
+        <v>367</v>
       </c>
       <c r="R41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S41" t="s">
+        <v>298</v>
+      </c>
+      <c r="U41" t="s">
+        <v>16</v>
+      </c>
+      <c r="V41" t="s">
+        <v>16</v>
+      </c>
+      <c r="W41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -5230,7 +5433,7 @@
         <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D42">
         <v>25</v>
@@ -5239,40 +5442,55 @@
         <v>104</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="H42" t="s">
+        <v>325</v>
+      </c>
+      <c r="G42" t="s">
+        <v>325</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I42" t="s">
+        <v>195</v>
+      </c>
+      <c r="J42" t="s">
+        <v>196</v>
+      </c>
+      <c r="K42" t="s">
         <v>197</v>
       </c>
-      <c r="I42" t="s">
-        <v>198</v>
-      </c>
-      <c r="J42" t="s">
-        <v>199</v>
-      </c>
-      <c r="K42" t="s">
-        <v>104</v>
-      </c>
       <c r="L42" t="s">
-        <v>337</v>
+        <v>104</v>
       </c>
       <c r="M42" t="s">
-        <v>321</v>
-      </c>
-      <c r="O42" t="s">
+        <v>318</v>
+      </c>
+      <c r="N42" t="s">
+        <v>319</v>
+      </c>
+      <c r="O42">
+        <v>1985</v>
+      </c>
+      <c r="P42" t="s">
         <v>172</v>
       </c>
-      <c r="Q42" t="s">
-        <v>104</v>
-      </c>
       <c r="R42" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S42" t="s">
+        <v>316</v>
+      </c>
+      <c r="U42" t="s">
+        <v>16</v>
+      </c>
+      <c r="V42" t="s">
+        <v>16</v>
+      </c>
+      <c r="W42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>99</v>
       </c>
@@ -5280,49 +5498,58 @@
         <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>323</v>
+        <v>198</v>
       </c>
       <c r="D43">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
         <v>104</v>
       </c>
       <c r="F43" t="s">
-        <v>328</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H43" t="s">
-        <v>128</v>
+        <v>199</v>
+      </c>
+      <c r="G43" t="s">
+        <v>199</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="I43" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="J43" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="K43" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="L43" t="s">
-        <v>338</v>
+        <v>104</v>
       </c>
       <c r="M43" t="s">
-        <v>290</v>
-      </c>
-      <c r="O43" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>104</v>
+        <v>201</v>
+      </c>
+      <c r="O43">
+        <v>1985</v>
       </c>
       <c r="R43" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S43" t="s">
+        <v>198</v>
+      </c>
+      <c r="U43" t="s">
+        <v>16</v>
+      </c>
+      <c r="V43" t="s">
+        <v>16</v>
+      </c>
+      <c r="W43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -5330,96 +5557,135 @@
         <v>82</v>
       </c>
       <c r="C44" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D44">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E44" t="s">
         <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="H44" t="s">
-        <v>128</v>
+        <v>93</v>
+      </c>
+      <c r="G44" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="I44" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="J44" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="K44" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="L44" t="s">
-        <v>339</v>
+        <v>104</v>
       </c>
       <c r="M44" t="s">
-        <v>290</v>
-      </c>
-      <c r="O44" t="s">
+        <v>335</v>
+      </c>
+      <c r="N44" t="s">
+        <v>319</v>
+      </c>
+      <c r="O44">
+        <v>2001</v>
+      </c>
+      <c r="P44" t="s">
         <v>172</v>
       </c>
-      <c r="Q44" t="s">
-        <v>104</v>
-      </c>
       <c r="R44" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="S44" t="s">
+        <v>320</v>
+      </c>
+      <c r="U44" t="s">
+        <v>16</v>
+      </c>
+      <c r="V44" t="s">
+        <v>57</v>
+      </c>
+      <c r="W44" t="s">
+        <v>57</v>
+      </c>
+      <c r="X44" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>99</v>
       </c>
       <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" t="s">
+        <v>321</v>
+      </c>
+      <c r="D45">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" t="s">
         <v>326</v>
       </c>
-      <c r="C45" t="s">
-        <v>325</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>104</v>
-      </c>
-      <c r="F45" t="s">
-        <v>329</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="H45" t="s">
-        <v>334</v>
+      <c r="G45" t="s">
+        <v>326</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="I45" t="s">
-        <v>335</v>
+        <v>128</v>
       </c>
       <c r="J45" t="s">
+        <v>134</v>
+      </c>
+      <c r="K45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" t="s">
+        <v>104</v>
+      </c>
+      <c r="M45" t="s">
         <v>336</v>
       </c>
-      <c r="K45" t="s">
-        <v>104</v>
-      </c>
-      <c r="L45" t="s">
-        <v>340</v>
-      </c>
-      <c r="M45" t="s">
-        <v>341</v>
-      </c>
-      <c r="O45" t="s">
+      <c r="N45" t="s">
+        <v>288</v>
+      </c>
+      <c r="O45">
+        <v>1989</v>
+      </c>
+      <c r="P45" t="s">
         <v>172</v>
       </c>
-      <c r="Q45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R45" t="s">
+        <v>104</v>
+      </c>
+      <c r="S45" t="s">
+        <v>321</v>
+      </c>
+      <c r="U45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V45" t="s">
+        <v>16</v>
+      </c>
+      <c r="W45" t="s">
+        <v>16</v>
+      </c>
+      <c r="X45" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -5427,42 +5693,74 @@
         <v>82</v>
       </c>
       <c r="C46" t="s">
-        <v>356</v>
+        <v>322</v>
+      </c>
+      <c r="D46">
+        <v>24</v>
       </c>
       <c r="E46" t="s">
         <v>104</v>
       </c>
       <c r="F46" t="s">
-        <v>357</v>
+        <v>95</v>
+      </c>
+      <c r="G46" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="I46" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="J46" t="s">
-        <v>199</v>
+        <v>134</v>
       </c>
       <c r="K46" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="L46" t="s">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="M46" t="s">
-        <v>321</v>
-      </c>
-      <c r="O46" t="s">
+        <v>337</v>
+      </c>
+      <c r="N46" t="s">
+        <v>288</v>
+      </c>
+      <c r="O46">
+        <v>1991</v>
+      </c>
+      <c r="P46" t="s">
         <v>172</v>
       </c>
-      <c r="Q46" t="s">
-        <v>104</v>
-      </c>
       <c r="R46" t="s">
-        <v>356</v>
+        <v>104</v>
+      </c>
+      <c r="S46" t="s">
+        <v>322</v>
+      </c>
+      <c r="U46" t="s">
+        <v>16</v>
+      </c>
+      <c r="V46" t="s">
+        <v>57</v>
+      </c>
+      <c r="W46" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R45">
-    <sortCondition ref="C2:C45"/>
+  <autoFilter ref="A1:U46" xr:uid="{29D658CB-784C-45A1-9FD5-F00CC052A358}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="WCVI"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:U46">
+    <sortCondition ref="B2:B46"/>
+    <sortCondition ref="C2:C46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>